<commit_message>
fix few statscan health region encoding issues
</commit_message>
<xml_diff>
--- a/health region lookup.xlsx
+++ b/health region lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://009co-my.sharepoint.com/personal/curtis_009co_onmicrosoft_com/Documents/www/ws_canadahr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="432" documentId="11_F25DC773A252ABDACC10484891D944A45ADE58E1" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2E2785F3-C039-49A0-A908-6387DE74B8F4}"/>
+  <xr:revisionPtr revIDLastSave="435" documentId="11_F25DC773A252ABDACC10484891D944A45ADE58E1" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C9CFDB61-A7E5-41D7-A231-457BE602F15E}"/>
   <bookViews>
-    <workbookView xWindow="4836" yWindow="276" windowWidth="17088" windowHeight="11448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5664" yWindow="528" windowWidth="17088" windowHeight="11448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hr_name_mapping" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="253">
   <si>
     <t>Abitibi-Témiscamingue</t>
   </si>
@@ -740,18 +740,12 @@
     <t>Région de la Côte-Nord</t>
   </si>
   <si>
-    <t>Région de la GaspésieÎles-de-la-Madeleine</t>
-  </si>
-  <si>
     <t>Région de la Mauricie et du Centre-du-Québec</t>
   </si>
   <si>
     <t>Région du Nord-du-Québec</t>
   </si>
   <si>
-    <t>Région du SaguenayLac-Saint-Jean</t>
-  </si>
-  <si>
     <t>Région des Terres-Cries-de-la-Baie-James</t>
   </si>
   <si>
@@ -795,6 +789,15 @@
   </si>
   <si>
     <t>Région de la Capitale-Nationale</t>
+  </si>
+  <si>
+    <t>Région de la Gaspésie Îles-de-la-Madeleine</t>
+  </si>
+  <si>
+    <t>Région du Saguenay Lac-Saint-Jean</t>
+  </si>
+  <si>
+    <t>Elgin-St. Thomas Health Unit</t>
   </si>
 </sst>
 </file>
@@ -1133,8 +1136,8 @@
   <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1252,7 +1255,7 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1340,7 +1343,7 @@
         <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1351,7 +1354,7 @@
         <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1362,7 +1365,7 @@
         <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1373,7 +1376,7 @@
         <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1384,7 +1387,7 @@
         <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1395,7 +1398,7 @@
         <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1406,7 +1409,7 @@
         <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1741,7 +1744,7 @@
         <v>87</v>
       </c>
       <c r="B55" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C55" t="s">
         <v>157</v>
@@ -1752,7 +1755,7 @@
         <v>87</v>
       </c>
       <c r="B56" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C56" t="s">
         <v>155</v>
@@ -1763,10 +1766,10 @@
         <v>87</v>
       </c>
       <c r="B57" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C57" t="s">
-        <v>138</v>
+        <v>252</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1950,7 +1953,7 @@
         <v>0</v>
       </c>
       <c r="C74" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1961,7 +1964,7 @@
         <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -1972,7 +1975,7 @@
         <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -2016,7 +2019,7 @@
         <v>16</v>
       </c>
       <c r="C80" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -2060,7 +2063,7 @@
         <v>34</v>
       </c>
       <c r="C84" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -2093,7 +2096,7 @@
         <v>39</v>
       </c>
       <c r="C87" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -2126,7 +2129,7 @@
         <v>56</v>
       </c>
       <c r="C90" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -2137,7 +2140,7 @@
         <v>63</v>
       </c>
       <c r="C91" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>